<commit_message>
saving the cleaned dataset to csv
</commit_message>
<xml_diff>
--- a/Dataset/TestDataset.xlsx
+++ b/Dataset/TestDataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\SpamCOVID-19\SpamCOVID-19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\GitHub\SpamCOVID-19\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -210,208 +210,6 @@
   </si>
   <si>
     <t>Scientists at AstraZeneca complain their work on a coronavirus vaccine keeps being delayed by Noddy Holder ringing up to ask if it will be ready by Christmas https://t.co/2lmYzTnAPx</t>
-  </si>
-  <si>
-    <t>Masks can help prevent the spread of #COVID19 when they are widely used in public. When you wear a mask you can help protect those around you. When others wear one they can help protect people around them incl. you. https://t.co/jkWwZTfWSS #WearAMask #DoYourPart #WorldMaskWeek https://t.co/O7FckRf1ks</t>
-  </si>
-  <si>
-    <t>132 new cases of #COVID19Nigeria; Lagos-52 Gombe-27 Plateau-17 Kwara-10 Enugu-9 Ogun-9 Katsina-3 Ekiti-2 Bauchi-1 Osun-1 Rivers-1 56388 confirmed 44337 discharged 1083 deaths https://t.co/Enpey5u7xh</t>
-  </si>
-  <si>
-    <t>Did You Already Have Coronavirus? Here’s A Simple Test https://t.co/PNbf76rsFF</t>
-  </si>
-  <si>
-    <t>RT @MoHFW_INDIA: #IndiaFightsCorona With high number of sustained recoveries India surges ahead with highest single day RECOVERY. Nearl…</t>
-  </si>
-  <si>
-    <t>Italy has surrendered to the coronavirus pandemic as all the measures to control COVID-19 have been exhausted.</t>
-  </si>
-  <si>
-    <t>President Trump Has Been Forced to Wear a Protective Medical Mask https://t.co/nrGTiXVrtV #donaldtrump #coronavirus #cia #fbi #iud</t>
-  </si>
-  <si>
-    <t>RT @EllenCutch: Coronavirus misinformation is moving offline. A reddit user posted this flyer to the site and told us it had been delive…</t>
-  </si>
-  <si>
-    <t>Orwell not dead but living under a bridge (continued) https://t.co/kL3j4vYwWP #government #toiletpaper #georgeorwell #coronavirus</t>
-  </si>
-  <si>
-    <t>Residents of York are asked what they think of a new government rule which allows people in England who may have #COVID19 to be fined up to £10000 if they fail to self-isolate. To read more click here: https://t.co/pqD1I8xgam https://t.co/QPgh3xlDIo</t>
-  </si>
-  <si>
-    <t>Central government has given permission for schools to re-open.</t>
-  </si>
-  <si>
-    <t>As of today there are a total of 1339 @ICMRDELHI approved labs for #COVID19 testing. These consist of 911 Govt &amp;amp; 428 Pvt labs: https://t.co/j4tAvyIcKc #CovidTesting #COVID__19 #COVID #Covid_19 #COVIDー19 #COVID19India #COVIDUpdates #coronavirus #CoronaUpdates #CoronavirusIndia https://t.co/Q0IuKceIFX</t>
-  </si>
-  <si>
-    <t>The government has come under pressure over a lack of availability of #COVID19 tests. Read more here: https://t.co/lMM9qgEryL https://t.co/KjwsinY5s1</t>
-  </si>
-  <si>
-    <t>Fewer kids are dying since the lockdown - A new white paper examines why.</t>
-  </si>
-  <si>
-    <t>More than 15 million cases of #COVID19 have now been reported to WHO and almost 620000 deaths. Although all countries have been affected we continue to see intense transmission in a relatively small group of countries-@DrTedros</t>
-  </si>
-  <si>
-    <t>Justin Trudeau Resigns Amidst Coronavirus Pandemic https://t.co/hKmcnbXSnB</t>
-  </si>
-  <si>
-    <t>George Soros is one of the people responsible for the new coronavirus born in a laboratory.</t>
-  </si>
-  <si>
-    <t>@JohnKin17583856 The sensitivity of the test is definitely something specialists are talking about. I have not seen a real number but I also haven’t looked that hard because we’ve been doing other things.-@alexismadrigal</t>
-  </si>
-  <si>
-    <t>Experts Call Out Claims That Cow Dung/Urine, Yoga, AYUSH Can Prevent Or Treat COVID-19</t>
-  </si>
-  <si>
-    <t>The main mode of transmission of #Novel #Coronavirus is through droplets and it is possible that infected smokers may blow droplets carrying the virus when they exhale. Regardless of #COVID19 you should steer clear of second-hand smoke as it may cause various health problems. https://t.co/aF3bZRlEve</t>
-  </si>
-  <si>
-    <t>An article claiming that "Bill Gates' vaccine" would modify human DNA.</t>
-  </si>
-  <si>
-    <t>RT @Surgeon_General: #DYK: #Handwashing remains one of the best ways to prevent the spread of viruses like #COVID19. Here are 5️⃣ things to…</t>
-  </si>
-  <si>
-    <t>According to the State Health Department #Haryana #COVID19 #RecoveryRate in #Gurugram is 86.7%: https://t.co/oZ9KCDajIJ #COVID19 #Covid_19 #COVIDー19 #CoronaUpdates #CoronavirusIndia #CoronaVirusUpdates #coronavirus #COVIDUpdates https://t.co/2Sp8yRRRWj</t>
-  </si>
-  <si>
-    <t>Our daily update is published. Sundays and Mondays are when we tend to see the numbers dip—and we see that today. Still: 62k cases rising hospitalizations and a large jump in deaths over last Sunday’s holiday numbers. The 7-day average is now back over 700. https://t.co/5hdQFxQ2OJ</t>
-  </si>
-  <si>
-    <t>Our total number of confirmed cases of COVID-19 is now 1431 which is the number we report to the World Health Organization.</t>
-  </si>
-  <si>
-    <t>Brazailian parliament went to a hospital that should take in COVID19 patients and found it was empty.</t>
-  </si>
-  <si>
-    <t>Multiple posts shared thousands of times on Facebook Twitter and YouTube claim that salt is an effective remedy against the novel coronavirus.</t>
-  </si>
-  <si>
-    <t>UN Secretary-General Antonio Guterres says the #COVID19 pandemic has "dramatically derailed" sustainable development goals and has "put into question" progress that was being made on the eradication of poverty and hunger. Latest world news: https://t.co/CDN8pokUbF https://t.co/TFzPdfFyRC</t>
-  </si>
-  <si>
-    <t>An Instagram post is claiming Covid-19 tests tainted with coronavirus have been in circulation for "many months".</t>
-  </si>
-  <si>
-    <t>Across the 21 states who report them we tracked 4468 hospitalizations the bulk in New York. But Louisiana and Florida also have growing numbers of hospitalizations.</t>
-  </si>
-  <si>
-    <t>Philippines Senators Grace Poe and Risa Hontiveros have been silent over the coronavirus crisis but were very vocal about the closure of ABS-CBN.</t>
-  </si>
-  <si>
-    <t>#IndiaFightsCorona: India’s Total Recoveries continue to rise cross 32.5 lakh today 5 States contribute 60% of total cases 62% of active cases and 70% of total fatality reported in India #StaySafe #IndiaWillWin https://t.co/KRn3GOaBNp</t>
-  </si>
-  <si>
-    <t>"The most important consequence of seeing COVID-19
-as a syndemic is to underline its social origins. The
-vulnerability of older citizens; Black, Asian, and minority
-ethnic communities; and key workers who are commonly
-poorly paid with fewer welfare protections..."</t>
-  </si>
-  <si>
-    <t>RT @COVIDNewsByMIB: #IndiaFightsCorona: @ICMRDELHI scales up Covid-19 testing capacity to 3 lakh tests per day in country. As of now tota…</t>
-  </si>
-  <si>
-    <t>A video shows an Italian doctor who says that nobody died from coronavirus in Italy that it's not more dangerous than a flu.</t>
-  </si>
-  <si>
-    <t>Seasonal influenza vaccination will be mandatory in Georgia this fall. COVID-19 mortality rates are significantly lower than the fatalities caused by other viruses.</t>
-  </si>
-  <si>
-    <t>We can now say there are 33 cases in the Mt Roskill Evangelical Fellowship group and 13 cases in the bereavement sub-cluster which includes the cases whose source of infection was the bereavement events.</t>
-  </si>
-  <si>
-    <t>There is no one in New Zealand receiving hospital-level care for COVID-19.⁣ ⁣ Yesterday our laboratories completed 2111 tests bringing the total number of tests completed to date to 280983. #covid19 #covid19nz #COVIDー19</t>
-  </si>
-  <si>
-    <t>As at 11:50 pm 19th April the breakdown of cases by state is: Lagos- 376 FCT- 88 Kano- 36 Osun- 20 Oyo- 16 Edo- 15 Ogun- 12 Kwara- 9 Katsina- 12 Bauchi- 7 Kaduna- 6 Akwa Ibom- 9 Delta- 4 Ekiti- 3 Ondo- 3 Enugu- 2 Rivers-2 Niger- 2 Benue- 1 Anambra- 1 Borno- 1 Jigawa- 2</t>
-  </si>
-  <si>
-    <t>The biggest change in the data is in the number of COVID-19 patients who are currently hospitalized. With the addition of Florida's 7k hospitalizations we’re now over 51000. We have not seen those numbers since the first week of May—and they do not seem likely to decline soon. https://t.co/tRvO4ypKGF</t>
-  </si>
-  <si>
-    <t>📢#CoronaVirusUpdates: 📍#COVID19 India Tracker (As on 7 September 2020 08:00 AM) ➡️Confirmed cases: 4204613 ➡️Recovered: 3250429 (77.3%)👍 ➡️Active cases: 882542 (21.0%) ➡️Deaths: 71642 (1.7%) #IndiaFightsCorona #IndiaWillWin #StaySafe Via @MoHFW_INDIA https://t.co/WVQslxqBPC</t>
-  </si>
-  <si>
-    <t>There is a person with coronavirus in Galicia on 2/4/20.</t>
-  </si>
-  <si>
-    <t>India has now tested more than 2 lakh samples/day for #COVID19! This has been enabled by @ICMRDelhi's commitment to set up over 1000 Laboratories and expanding testing mechanisms. For details visit: https://t.co/FQhg5M5xrN #ICMRFightsCOVID19 #IndiaFightsCorona @MoHFW_INDIA https://t.co/rDkcvFbhUS</t>
-  </si>
-  <si>
-    <t>Claim that the Jordanian Health minister says COVID-19 is a conspiracy in a video.</t>
-  </si>
-  <si>
-    <t>Pregnant women with COVID have a 25% higher rate of premature births. https://t.co/g1hScYwGpr</t>
-  </si>
-  <si>
-    <t>@WHO Solidarity Trials are also underway in many countries. Once these projects are complete controlling #COVID19 effectively will be easier due to the availability of proper medicines vaccines etc. as did to control various infectious diseases across the world.</t>
-  </si>
-  <si>
-    <t>COVID-19 update: There are no new cases of COVID-19 to report in New Zealand today. It has been 99 days since the last case of COVID-19 was acquired locally from an unknown source.</t>
-  </si>
-  <si>
-    <t>Compare the number of completed tests reported by New Mexico a state with a population 19 times smaller than California’s. These numbers should not even be close and yet they are. https://t.co/tzB9fZM6FP</t>
-  </si>
-  <si>
-    <t>All 12 cases in the community are Auckland based. All are connected to the existing outbreak as close contacts of cases already reported. 2 of the new cases are household contacts of a previously reported case that is still under investigation - the GP from Mt Wellington.</t>
-  </si>
-  <si>
-    <t>A precautionary message that one can catch fire due to hand sanitizer as it has a high amount of alcohol. The message also shows the hands of a lady who after applying sanitizer went near the stove and ended up burning her hands.</t>
-  </si>
-  <si>
-    <t>That brings New Zealand’s total number of active cases to 14 all are in managed isolation or quarantine facilities. There are no cases in the community.  NZ's total number of confirmed cases of COVID-19 is now 1170 which is the number we report to the WHO.</t>
-  </si>
-  <si>
-    <t>Says Rudy Giuliani "bought $2M in shares of Novartis, a primary supplier of hydroxychloroquine" in early February.</t>
-  </si>
-  <si>
-    <t>_A student from Pondicherry University in India has found a home remedy for COVID-19 that has been accepted by World Health Organization (WHO)._</t>
-  </si>
-  <si>
-    <t>Footballer Ronaldo is turning his hotels into COVID-19 hospitals.</t>
-  </si>
-  <si>
-    <t>#CoronaVirusUpdates India records Highest ever single day peak of 63631 #COVID19 recoveries. #IndiaFightsCorona as Total recoveries cross 22 lakh. Recoveries exceed the active cases by more than 15 lakh. https://t.co/XBY3Er8K0P https://t.co/VDQSv7xVUB</t>
-  </si>
-  <si>
-    <t>Do you have a cough fever or runny nose? If these symptoms came on suddenly there’s a good chance you could have #flu. Watch to find out what you should do next to #fightflu. https://t.co/fp3aSjumw4</t>
-  </si>
-  <si>
-    <t>President Trump Says Pandas Are Responsible For Covid-19 https://t.co/mgan5G2oY8 #donaldtrump #china #coronavirus #zoo #pandas</t>
-  </si>
-  <si>
-    <t>As of today there are 23917 active #COVID19 cases in #Mumbai District #Maharastra: https://t.co/6CcqIYgbXL @MoHFW_INDIA @drharshvardhan @DrHVoffice @MantralayaRoom #COVID__19 #Covid_19 #COVIDー19 #CoronaUpdatesInIndia #Coronavirus #CoronaVirusUpdates #CoronavirusPandemic https://t.co/k6ICon5kZ6</t>
-  </si>
-  <si>
-    <t>Public Health England's weekly #coronavirus report shows a rise of almost 23% in rhinovirus infections which include the common cold in the last week https://t.co/N6jzZYU7lJ</t>
-  </si>
-  <si>
-    <t>This is an image of a suspected coronavirus vaccine causing COVID-19.</t>
-  </si>
-  <si>
-    <t>Some people are more likely than others to become severely ill from #COVID19 which means that they may require hospitalization intensive care or a ventilator to help them breathe. Some severely ill people may die. Learn more. https://t.co/15lxFaQqX7 https://t.co/MAnreCAV8G</t>
-  </si>
-  <si>
-    <t>Camila Pitanga Brazilian actress contracted COVID-19 but said she caught malaria so she could take chloroquine without admitting she was wrong.</t>
-  </si>
-  <si>
-    <t>The new coronavirus "causes sudden death syndrome."</t>
-  </si>
-  <si>
-    <t>#IndiaFightsCorona: 📍 Increasing gap between #COVID19 Recovered &amp;amp; Active cases of India (May 04 2020 to September 11 2020)👇 #StaySafe #IndiaWillWin https://t.co/FFJ4DKyspR</t>
-  </si>
-  <si>
-    <t>Coronavirus parties can have deadly consequences. https://t.co/WTriJWJu9T</t>
-  </si>
-  <si>
-    <t>Cabinet Office Minister Michael Gove says 'there's going to be a shift of emphasis' on working from home in the new #COVID19 restrictions. #KayBurley Get the latest #coronavirus news: https://t.co/hk8hrup8AY https://t.co/q8Btm4YE1P</t>
-  </si>
-  <si>
-    <t>@James_Gross Well they are now reporting quite effectively. It's just they refuse to put their numbers in a table or dashboard for reasons that are beyond me.</t>
   </si>
 </sst>
 </file>
@@ -784,11 +582,11 @@
   </sheetPr>
   <dimension ref="A1:C6421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C117" sqref="A52:C117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="192.5703125" customWidth="1"/>
   </cols>
@@ -1355,730 +1153,334 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>54</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>56</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>57</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <v>62</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <v>63</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
-        <v>64</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
-        <v>65</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
-        <v>66</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
-        <v>67</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
-        <v>68</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
-        <v>69</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
-        <v>70</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
-        <v>71</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
-        <v>72</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
-        <v>73</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
-        <v>74</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
-        <v>75</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
-        <v>76</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1">
-        <v>77</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1">
-        <v>78</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1">
-        <v>79</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1">
-        <v>80</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1">
-        <v>81</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A83" s="1">
-        <v>82</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A84" s="1">
-        <v>83</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
     </row>
     <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="1">
-        <v>84</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="1">
-        <v>85</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="1">
-        <v>86</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="1">
-        <v>87</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
-        <v>88</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
     </row>
     <row r="90" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A90" s="1">
-        <v>89</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
     </row>
     <row r="91" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="1">
-        <v>90</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
     </row>
     <row r="92" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A92" s="1">
-        <v>91</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
     </row>
     <row r="93" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="1">
-        <v>92</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A94" s="1">
-        <v>93</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
     </row>
     <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="1">
-        <v>94</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A96" s="1">
-        <v>95</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
     </row>
     <row r="97" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A97" s="1">
-        <v>96</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
     </row>
     <row r="98" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A98" s="1">
-        <v>97</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
     </row>
     <row r="99" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A99" s="1">
-        <v>98</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A100" s="1">
-        <v>99</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
-        <v>100</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A102" s="1">
-        <v>101</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A103" s="1">
-        <v>102</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
     </row>
     <row r="104" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A104" s="1">
-        <v>103</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
     </row>
     <row r="105" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A105" s="1">
-        <v>104</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
     </row>
     <row r="106" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A106" s="1">
-        <v>105</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
     </row>
     <row r="107" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A107" s="1">
-        <v>106</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A108" s="1">
-        <v>107</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
-        <v>108</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
     </row>
     <row r="110" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A110" s="1">
-        <v>109</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
     </row>
     <row r="111" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A111" s="1">
-        <v>110</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
     </row>
     <row r="112" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A112" s="1">
-        <v>111</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
     </row>
     <row r="113" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A113" s="1">
-        <v>112</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
     </row>
     <row r="114" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A114" s="1">
-        <v>113</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
     </row>
     <row r="115" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A115" s="1">
-        <v>114</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
     </row>
     <row r="116" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A116" s="1">
-        <v>115</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
     </row>
     <row r="117" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A117" s="1">
-        <v>116</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
     </row>
     <row r="118" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
@@ -33618,12 +33020,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000E78AF11E754646AA592EDA218D5F94" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="cb9d5243d5e912349fe1a4d4c8d6cb85">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2cc73722-0bc8-4945-a9ce-9fd4614c5ce5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="192d0e71e7dd23fb68c821970bc25c76" ns2:_="">
     <xsd:import namespace="2cc73722-0bc8-4945-a9ce-9fd4614c5ce5"/>
@@ -33755,6 +33151,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5076AB0-C6EB-4927-BE84-F0149EAF5898}">
   <ds:schemaRefs>
@@ -33764,15 +33166,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BE87362-4083-4B73-8FBF-F163F5598C36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6200F3D-D995-4719-869F-758E09F7963E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33788,4 +33181,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BE87362-4083-4B73-8FBF-F163F5598C36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>